<commit_message>
outliers removed and prior of ql for FRV off
</commit_message>
<xml_diff>
--- a/project1_mess3/data/data.xlsx
+++ b/project1_mess3/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitytasmania-my.sharepoint.com/personal/hoang_nguyen0_utas_edu_au/Documents/HOANG.Ng84/Education/Hoang.MUN20/Required courses/Fish 6005/labs/F6005/project1_mess3/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="361" documentId="13_ncr:1_{D500D30F-546F-4815-8672-29DB70640AF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F8D6C436-C3CA-4665-9973-7CF9B169D851}"/>
+  <xr:revisionPtr revIDLastSave="362" documentId="13_ncr:1_{D500D30F-546F-4815-8672-29DB70640AF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B1337EAD-A066-4D72-940A-6FBEA5C4A91C}"/>
   <bookViews>
-    <workbookView xWindow="29610" yWindow="-120" windowWidth="28110" windowHeight="16440" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29610" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="catch" sheetId="1" r:id="rId1"/>
@@ -13853,8 +13853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F36F9BE8-C929-4F96-9B30-5825B67EEBF8}">
   <dimension ref="A1:AE46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16574,7 +16574,7 @@
       <c r="R29">
         <v>2</v>
       </c>
-      <c r="S29">
+      <c r="S29" s="2">
         <v>4</v>
       </c>
       <c r="T29">
@@ -16669,7 +16669,7 @@
       <c r="R30">
         <v>1</v>
       </c>
-      <c r="S30">
+      <c r="S30" s="2">
         <v>2</v>
       </c>
       <c r="T30">
@@ -29711,7 +29711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{511C3F20-75F5-4DF9-97FC-97DCB653C4F0}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:O31"/>
     </sheetView>
   </sheetViews>
@@ -40379,6 +40379,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001981DE4BE955644C849A34F962AE4E4D" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14093cb3fb38152639c28edb59c9f9fc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f5aaa703-530c-4b46-9523-3fe71b6b9bfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5be1f5ce6025993eb3115f090e11ba15" ns2:_="">
     <xsd:import namespace="f5aaa703-530c-4b46-9523-3fe71b6b9bfd"/>
@@ -40536,15 +40545,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F7EC5D8-7144-4784-A799-CDA3F5712AB2}">
   <ds:schemaRefs>
@@ -40555,6 +40555,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE5E38A4-DB89-4A72-AFF8-F8BA174B3BB0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3991913-2DA6-4EA6-85A3-F4D8BB1FA9CE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -40570,12 +40578,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE5E38A4-DB89-4A72-AFF8-F8BA174B3BB0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>